<commit_message>
Explanations of lubm1 with 100K rows
</commit_message>
<xml_diff>
--- a/src/main/resources/AlgoRunLubm1.xlsx
+++ b/src/main/resources/AlgoRunLubm1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Research\MyPapers\002-Preparation\2020_ISJournal2020\raxonDB\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\pvassil\RESEARCH\EclipseForResearch\raxonDB\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE87329E-3B56-41BE-B734-3215C138AC7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39422B9F-77DD-426E-AD4B-964F294E6F21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A8C81FE-15A4-4CE0-A6F7-C85EE98DE310}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1A8C81FE-15A4-4CE0-A6F7-C85EE98DE310}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -257,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -272,6 +272,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -287,6 +288,207 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>2444750</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29DDAD34-773E-45F4-A595-0C1817762BD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13843000" y="2317750"/>
+          <a:ext cx="2301875" cy="3063875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t>[[0, 2, 4, 5, 6, 7, 8, 9, 10, 11],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 19, 21, 26],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 19, 27, 28],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 18, 19, 20],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 19, 21],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 1],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [22, 23],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 3],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 19, 26],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 19, 27],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 2, 4, 5, 6, 7, 8, 9, 10],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 19, 29],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 19, 30],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 19],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 19, 27, 28, 30],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 2, 5, 9, 10, 13, 14, 15],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 19, 27, 28, 29],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 2, 5, 9, 10, 13, 14, 15, 17],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 2, 3],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 24, 25],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 2, 9, 10, 13, 14, 15],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1050"/>
+            <a:t> [0, 2, 4, 5, 6, 7, 8, 9, 10, 11, 12]]  </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -588,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDE4215-35D5-492D-ADB9-88058B82996C}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:Q1"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,12 +802,12 @@
     <col min="5" max="5" width="31" customWidth="1"/>
     <col min="6" max="6" width="20.140625" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
     <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
     <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="13" max="13" width="0.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -953,10 +1155,10 @@
       <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="8">
         <v>37511</v>
       </c>
       <c r="D12" s="2">
@@ -992,10 +1194,10 @@
       <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="8">
         <v>11047</v>
       </c>
       <c r="D13" s="2"/>
@@ -1021,10 +1223,10 @@
       <c r="A14" s="1">
         <v>11</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="8">
         <v>13727</v>
       </c>
       <c r="D14" s="2"/>
@@ -1108,10 +1310,10 @@
       <c r="A17" s="1">
         <v>14</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="8">
         <v>22632</v>
       </c>
       <c r="D17" s="2">
@@ -1469,5 +1671,11 @@
     <mergeCell ref="N1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="99" orientation="landscape" r:id="rId1"/>
+  <colBreaks count="2" manualBreakCount="2">
+    <brk id="8" max="1048575" man="1"/>
+    <brk id="13" max="1048575" man="1"/>
+  </colBreaks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>